<commit_message>
put both the transpose and not
</commit_message>
<xml_diff>
--- a/Thresholding/Results/results_table.xlsx
+++ b/Thresholding/Results/results_table.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="285">
   <si>
     <t>Row</t>
   </si>
@@ -355,6 +355,348 @@
   </si>
   <si>
     <t>MatchPercentage</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>BJ_Y1</t>
+  </si>
+  <si>
+    <t>BJ_Y2</t>
+  </si>
+  <si>
+    <t>BJ_Y3</t>
+  </si>
+  <si>
+    <t>BJ_OLD_1</t>
+  </si>
+  <si>
+    <t>BJ_OLD_2</t>
+  </si>
+  <si>
+    <t>BJ_OLD_3</t>
+  </si>
+  <si>
+    <t>IMR90_Y1</t>
+  </si>
+  <si>
+    <t>IMR90_Y2</t>
+  </si>
+  <si>
+    <t>IMR90_Y3</t>
+  </si>
+  <si>
+    <t>IMR90_O1</t>
+  </si>
+  <si>
+    <t>IMR90_O2</t>
+  </si>
+  <si>
+    <t>IMR90_O3</t>
+  </si>
+  <si>
+    <t>WI_38_Y1</t>
+  </si>
+  <si>
+    <t>WI_38_Y2</t>
+  </si>
+  <si>
+    <t>WI_38_Y3</t>
+  </si>
+  <si>
+    <t>WI_38_O1</t>
+  </si>
+  <si>
+    <t>WI_38_O2</t>
+  </si>
+  <si>
+    <t>WI_38_O3</t>
+  </si>
+  <si>
+    <t>HFF_PD16_1</t>
+  </si>
+  <si>
+    <t>HFF_PD16_2</t>
+  </si>
+  <si>
+    <t>HFF_PD16_3</t>
+  </si>
+  <si>
+    <t>HFF_PD74_1</t>
+  </si>
+  <si>
+    <t>HFF_PD74_2</t>
+  </si>
+  <si>
+    <t>HFF_PD74_3</t>
+  </si>
+  <si>
+    <t>MRC_5_PD32_1</t>
+  </si>
+  <si>
+    <t>MRC_5_PD32_2</t>
+  </si>
+  <si>
+    <t>MRC_5_PD32_3</t>
+  </si>
+  <si>
+    <t>MRC_5_PD72_1</t>
+  </si>
+  <si>
+    <t>MRC_5_PD72_2</t>
+  </si>
+  <si>
+    <t>MRC_5_PD72_3</t>
+  </si>
+  <si>
+    <t>HFF_PD26_1</t>
+  </si>
+  <si>
+    <t>HFF_PD26_2</t>
+  </si>
+  <si>
+    <t>HFF_PD26_3</t>
+  </si>
+  <si>
+    <t>HFF_PD46_1</t>
+  </si>
+  <si>
+    <t>HFF_PD46_2</t>
+  </si>
+  <si>
+    <t>HFF_PD46_3</t>
+  </si>
+  <si>
+    <t>HFF_PD64_1</t>
+  </si>
+  <si>
+    <t>HFF_PD64_2</t>
+  </si>
+  <si>
+    <t>HFF_PD64_3</t>
+  </si>
+  <si>
+    <t>MRC_5_PD42_1</t>
+  </si>
+  <si>
+    <t>MRC_5_PD42_2</t>
+  </si>
+  <si>
+    <t>MRC_5_PD42_3</t>
+  </si>
+  <si>
+    <t>MRC_5_PD52_1</t>
+  </si>
+  <si>
+    <t>MRC_5_PD52_2</t>
+  </si>
+  <si>
+    <t>MRC_5_PD52_3</t>
+  </si>
+  <si>
+    <t>MRC_5_PD62_1</t>
+  </si>
+  <si>
+    <t>MRC_5_PD62_2</t>
+  </si>
+  <si>
+    <t>MRC_5_PD62_3</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LG</t>
+  </si>
+  <si>
+    <t>Var4</t>
+  </si>
+  <si>
+    <t>HK_R_acc_G</t>
+  </si>
+  <si>
+    <t>HK_R_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_R_acc_LG</t>
+  </si>
+  <si>
+    <t>HK_R_acc_SD</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>BJ_Y1</t>
+  </si>
+  <si>
+    <t>BJ_Y2</t>
+  </si>
+  <si>
+    <t>BJ_Y3</t>
+  </si>
+  <si>
+    <t>BJ_OLD_1</t>
+  </si>
+  <si>
+    <t>BJ_OLD_2</t>
+  </si>
+  <si>
+    <t>BJ_OLD_3</t>
+  </si>
+  <si>
+    <t>IMR90_Y1</t>
+  </si>
+  <si>
+    <t>IMR90_Y2</t>
+  </si>
+  <si>
+    <t>IMR90_Y3</t>
+  </si>
+  <si>
+    <t>IMR90_O1</t>
+  </si>
+  <si>
+    <t>IMR90_O2</t>
+  </si>
+  <si>
+    <t>IMR90_O3</t>
+  </si>
+  <si>
+    <t>WI_38_Y1</t>
+  </si>
+  <si>
+    <t>WI_38_Y2</t>
+  </si>
+  <si>
+    <t>WI_38_Y3</t>
+  </si>
+  <si>
+    <t>WI_38_O1</t>
+  </si>
+  <si>
+    <t>WI_38_O2</t>
+  </si>
+  <si>
+    <t>WI_38_O3</t>
+  </si>
+  <si>
+    <t>HFF_PD16_1</t>
+  </si>
+  <si>
+    <t>HFF_PD16_2</t>
+  </si>
+  <si>
+    <t>HFF_PD16_3</t>
+  </si>
+  <si>
+    <t>HFF_PD74_1</t>
+  </si>
+  <si>
+    <t>HFF_PD74_2</t>
+  </si>
+  <si>
+    <t>HFF_PD74_3</t>
+  </si>
+  <si>
+    <t>MRC_5_PD32_1</t>
+  </si>
+  <si>
+    <t>MRC_5_PD32_2</t>
+  </si>
+  <si>
+    <t>MRC_5_PD32_3</t>
+  </si>
+  <si>
+    <t>MRC_5_PD72_1</t>
+  </si>
+  <si>
+    <t>MRC_5_PD72_2</t>
+  </si>
+  <si>
+    <t>MRC_5_PD72_3</t>
+  </si>
+  <si>
+    <t>HFF_PD26_1</t>
+  </si>
+  <si>
+    <t>HFF_PD26_2</t>
+  </si>
+  <si>
+    <t>HFF_PD26_3</t>
+  </si>
+  <si>
+    <t>HFF_PD46_1</t>
+  </si>
+  <si>
+    <t>HFF_PD46_2</t>
+  </si>
+  <si>
+    <t>HFF_PD46_3</t>
+  </si>
+  <si>
+    <t>HFF_PD64_1</t>
+  </si>
+  <si>
+    <t>HFF_PD64_2</t>
+  </si>
+  <si>
+    <t>HFF_PD64_3</t>
+  </si>
+  <si>
+    <t>MRC_5_PD42_1</t>
+  </si>
+  <si>
+    <t>MRC_5_PD42_2</t>
+  </si>
+  <si>
+    <t>MRC_5_PD42_3</t>
+  </si>
+  <si>
+    <t>MRC_5_PD52_1</t>
+  </si>
+  <si>
+    <t>MRC_5_PD52_2</t>
+  </si>
+  <si>
+    <t>MRC_5_PD52_3</t>
+  </si>
+  <si>
+    <t>MRC_5_PD62_1</t>
+  </si>
+  <si>
+    <t>MRC_5_PD62_2</t>
+  </si>
+  <si>
+    <t>MRC_5_PD62_3</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_G_acc_LG</t>
+  </si>
+  <si>
+    <t>Var4</t>
+  </si>
+  <si>
+    <t>HK_R_acc_G</t>
+  </si>
+  <si>
+    <t>HK_R_acc_LT</t>
+  </si>
+  <si>
+    <t>HK_R_acc_LG</t>
+  </si>
+  <si>
+    <t>HK_R_acc_SD</t>
   </si>
   <si>
     <t>Row</t>
@@ -587,36 +929,36 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>163</v>
+        <v>277</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>164</v>
+        <v>278</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>165</v>
+        <v>279</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>166</v>
+        <v>280</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>167</v>
+        <v>281</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>168</v>
+        <v>282</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>169</v>
+        <v>283</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>170</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>115</v>
+        <v>229</v>
       </c>
       <c r="B2" s="0">
         <v>52.548330404217921</v>
@@ -645,7 +987,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>116</v>
+        <v>230</v>
       </c>
       <c r="B3" s="0">
         <v>52.3725834797891</v>
@@ -674,7 +1016,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>117</v>
+        <v>231</v>
       </c>
       <c r="B4" s="0">
         <v>52.3725834797891</v>
@@ -703,7 +1045,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>118</v>
+        <v>232</v>
       </c>
       <c r="B5" s="0">
         <v>51.845342706502642</v>
@@ -732,7 +1074,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>119</v>
+        <v>233</v>
       </c>
       <c r="B6" s="0">
         <v>51.318101933216163</v>
@@ -761,7 +1103,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>120</v>
+        <v>234</v>
       </c>
       <c r="B7" s="0">
         <v>51.66959578207382</v>
@@ -790,7 +1132,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>121</v>
+        <v>235</v>
       </c>
       <c r="B8" s="0">
         <v>53.954305799648509</v>
@@ -819,7 +1161,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>122</v>
+        <v>236</v>
       </c>
       <c r="B9" s="0">
         <v>53.251318101933222</v>
@@ -848,7 +1190,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>123</v>
+        <v>237</v>
       </c>
       <c r="B10" s="0">
         <v>53.251318101933222</v>
@@ -877,7 +1219,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>124</v>
+        <v>238</v>
       </c>
       <c r="B11" s="0">
         <v>53.427065026362044</v>
@@ -906,7 +1248,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>125</v>
+        <v>239</v>
       </c>
       <c r="B12" s="0">
         <v>53.075571177504386</v>
@@ -935,7 +1277,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>126</v>
+        <v>240</v>
       </c>
       <c r="B13" s="0">
         <v>52.899824253075565</v>
@@ -964,7 +1306,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>127</v>
+        <v>241</v>
       </c>
       <c r="B14" s="0">
         <v>54.305799648506145</v>
@@ -993,7 +1335,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>128</v>
+        <v>242</v>
       </c>
       <c r="B15" s="0">
         <v>54.481546572934967</v>
@@ -1022,7 +1364,7 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>129</v>
+        <v>243</v>
       </c>
       <c r="B16" s="0">
         <v>54.305799648506145</v>
@@ -1051,7 +1393,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>130</v>
+        <v>244</v>
       </c>
       <c r="B17" s="0">
         <v>52.724077328646743</v>
@@ -1080,7 +1422,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>131</v>
+        <v>245</v>
       </c>
       <c r="B18" s="0">
         <v>53.075571177504386</v>
@@ -1109,7 +1451,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>132</v>
+        <v>246</v>
       </c>
       <c r="B19" s="0">
         <v>52.548330404217921</v>
@@ -1138,7 +1480,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>133</v>
+        <v>247</v>
       </c>
       <c r="B20" s="0">
         <v>53.251318101933222</v>
@@ -1167,7 +1509,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>134</v>
+        <v>248</v>
       </c>
       <c r="B21" s="0">
         <v>53.075571177504386</v>
@@ -1196,7 +1538,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>135</v>
+        <v>249</v>
       </c>
       <c r="B22" s="0">
         <v>53.427065026362044</v>
@@ -1225,7 +1567,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>136</v>
+        <v>250</v>
       </c>
       <c r="B23" s="0">
         <v>51.142355008787341</v>
@@ -1254,7 +1596,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>137</v>
+        <v>251</v>
       </c>
       <c r="B24" s="0">
         <v>50.087873462214418</v>
@@ -1283,7 +1625,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>138</v>
+        <v>252</v>
       </c>
       <c r="B25" s="0">
         <v>51.142355008787341</v>
@@ -1312,7 +1654,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>139</v>
+        <v>253</v>
       </c>
       <c r="B26" s="0">
         <v>52.899824253075565</v>
@@ -1341,7 +1683,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>140</v>
+        <v>254</v>
       </c>
       <c r="B27" s="0">
         <v>52.724077328646743</v>
@@ -1370,7 +1712,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>141</v>
+        <v>255</v>
       </c>
       <c r="B28" s="0">
         <v>53.602811950790866</v>
@@ -1399,7 +1741,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>142</v>
+        <v>256</v>
       </c>
       <c r="B29" s="0">
         <v>54.657293497363803</v>
@@ -1428,7 +1770,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>143</v>
+        <v>257</v>
       </c>
       <c r="B30" s="0">
         <v>53.954305799648509</v>
@@ -1457,7 +1799,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>144</v>
+        <v>258</v>
       </c>
       <c r="B31" s="0">
         <v>54.657293497363803</v>
@@ -1486,7 +1828,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>145</v>
+        <v>259</v>
       </c>
       <c r="B32" s="0">
         <v>50.615114235500883</v>
@@ -1515,7 +1857,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>146</v>
+        <v>260</v>
       </c>
       <c r="B33" s="0">
         <v>51.66959578207382</v>
@@ -1544,7 +1886,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>147</v>
+        <v>261</v>
       </c>
       <c r="B34" s="0">
         <v>51.845342706502642</v>
@@ -1573,7 +1915,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>148</v>
+        <v>262</v>
       </c>
       <c r="B35" s="0">
         <v>52.196836555360285</v>
@@ -1602,7 +1944,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>149</v>
+        <v>263</v>
       </c>
       <c r="B36" s="0">
         <v>51.66959578207382</v>
@@ -1631,7 +1973,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>150</v>
+        <v>264</v>
       </c>
       <c r="B37" s="0">
         <v>56.063268892794369</v>
@@ -1660,7 +2002,7 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>151</v>
+        <v>265</v>
       </c>
       <c r="B38" s="0">
         <v>51.142355008787341</v>
@@ -1689,7 +2031,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>152</v>
+        <v>266</v>
       </c>
       <c r="B39" s="0">
         <v>51.845342706502642</v>
@@ -1718,7 +2060,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>153</v>
+        <v>267</v>
       </c>
       <c r="B40" s="0">
         <v>51.318101933216163</v>
@@ -1747,7 +2089,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>154</v>
+        <v>268</v>
       </c>
       <c r="B41" s="0">
         <v>52.899824253075565</v>
@@ -1776,7 +2118,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>155</v>
+        <v>269</v>
       </c>
       <c r="B42" s="0">
         <v>53.427065026362044</v>
@@ -1805,7 +2147,7 @@
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>156</v>
+        <v>270</v>
       </c>
       <c r="B43" s="0">
         <v>53.954305799648509</v>
@@ -1834,7 +2176,7 @@
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>157</v>
+        <v>271</v>
       </c>
       <c r="B44" s="0">
         <v>53.427065026362044</v>
@@ -1863,7 +2205,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>158</v>
+        <v>272</v>
       </c>
       <c r="B45" s="0">
         <v>52.3725834797891</v>
@@ -1892,7 +2234,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>159</v>
+        <v>273</v>
       </c>
       <c r="B46" s="0">
         <v>52.548330404217921</v>
@@ -1921,7 +2263,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>160</v>
+        <v>274</v>
       </c>
       <c r="B47" s="0">
         <v>51.845342706502642</v>
@@ -1950,7 +2292,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>161</v>
+        <v>275</v>
       </c>
       <c r="B48" s="0">
         <v>54.481546572934967</v>
@@ -1979,7 +2321,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>162</v>
+        <v>276</v>
       </c>
       <c r="B49" s="0">
         <v>53.251318101933222</v>

</xml_diff>